<commit_message>
Only one exception tests fail
</commit_message>
<xml_diff>
--- a/data/ClueLayout.xlsx
+++ b/data/ClueLayout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leviortega/eclipse-workspace/ClueGame/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D169EA4-F069-9048-BFDA-0982C91C0A52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A11C677-8724-1B4B-A819-1655D059078A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16540" xr2:uid="{45C9F756-0EF2-7849-ADF8-7DE35EDE649F}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{1C509876-B554-0446-B4E9-CBA3C8A3C97C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="37">
   <si>
     <t>J</t>
   </si>
@@ -78,73 +78,64 @@
     <t>J*</t>
   </si>
   <si>
-    <t>N#</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>N*</t>
-  </si>
-  <si>
     <t>P#</t>
   </si>
   <si>
     <t>P*</t>
   </si>
   <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>S#</t>
+  </si>
+  <si>
+    <t>T*</t>
+  </si>
+  <si>
+    <t>T#</t>
+  </si>
+  <si>
+    <t>S*</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>Rv</t>
+  </si>
+  <si>
     <t>G</t>
   </si>
   <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>S#</t>
+    <t>O#</t>
+  </si>
+  <si>
+    <t>H#</t>
+  </si>
+  <si>
+    <t>O*</t>
   </si>
   <si>
     <t>G*</t>
   </si>
   <si>
+    <t>H*</t>
+  </si>
+  <si>
     <t>G#</t>
   </si>
   <si>
-    <t>S*</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>Rv</t>
-  </si>
-  <si>
-    <t>O#</t>
-  </si>
-  <si>
-    <t>H#</t>
-  </si>
-  <si>
-    <t>O*</t>
-  </si>
-  <si>
-    <t>H*</t>
-  </si>
-  <si>
     <t>HB</t>
   </si>
   <si>
     <t>GJ</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>T*</t>
-  </si>
-  <si>
-    <t>T#</t>
   </si>
 </sst>
 </file>
@@ -524,11 +515,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F03917-8A77-8547-824C-42C4669A202D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B7F116-7830-D441-8D6C-C8A95CF0130A}">
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1141,14 +1132,14 @@
       <c r="E9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>18</v>
+      <c r="F9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>3</v>
@@ -1215,17 +1206,17 @@
       <c r="E10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>18</v>
+      <c r="F10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>2</v>
@@ -1246,7 +1237,7 @@
         <v>3</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="Q10" s="1" t="s">
         <v>8</v>
@@ -1289,44 +1280,44 @@
       <c r="E11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="R11" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="O11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="S11" s="1" t="s">
         <v>8</v>
@@ -1497,28 +1488,28 @@
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>3</v>
@@ -1548,51 +1539,51 @@
         <v>3</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="V14" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="X14" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>3</v>
@@ -1622,51 +1613,51 @@
         <v>3</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="V15" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="X15" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>3</v>
@@ -1696,51 +1687,51 @@
         <v>3</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="V16" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="W16" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="X16" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>3</v>
@@ -1770,51 +1761,51 @@
         <v>11</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="U17" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="V17" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="W17" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="X17" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>15</v>
@@ -1844,25 +1835,25 @@
         <v>3</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="V18" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="W18" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="X18" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.2">
@@ -1941,16 +1932,16 @@
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>15</v>
@@ -1974,7 +1965,7 @@
         <v>3</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="M20" s="3" t="s">
         <v>15</v>
@@ -1995,60 +1986,60 @@
         <v>3</v>
       </c>
       <c r="S20" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="V20" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="W20" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="X20" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>3</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="M21" s="3" t="s">
         <v>3</v>
@@ -2066,173 +2057,173 @@
         <v>3</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="U21" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="V21" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="W21" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="X21" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="U22" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M22" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="N22" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="O22" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="P22" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q22" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="R22" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="S22" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="T22" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U22" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="V22" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="W22" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="X22" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M23" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="N23" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="O23" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="P23" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q23" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="R23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="S23" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="T23" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="U23" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="V23" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="W23" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="X23" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.2">
@@ -2240,40 +2231,40 @@
         <v>35</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>3</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="N24" s="3" t="s">
         <v>3</v>
@@ -2288,22 +2279,22 @@
         <v>3</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="T24" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="U24" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="V24" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="W24" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="X24" s="1" t="s">
         <v>36</v>

</xml_diff>